<commit_message>
wrote tests for stacking smaller grid widths and standard rectangles to fill the grid. Stacking standard rectangles doesnt work yet.
</commit_message>
<xml_diff>
--- a/tests/test_paklijsten/paklijst_kokos.xlsx
+++ b/tests/test_paklijsten/paklijst_kokos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\HDS\2d_rectangle_packing\tests\test_paklijsten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89527E83-8B08-4D19-BF56-3CBEACAF07AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4BD391-7719-42D4-9EC8-26FF5E45C30C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paklijst_zonder_opmaak" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Aantal</t>
   </si>
@@ -71,9 +71,6 @@
 Rolbreedte 200 cm_x000D_
 Breedte: 197cm, Lengte: 105 cm_x000D_
 </t>
-  </si>
-  <si>
-    <t>197</t>
   </si>
   <si>
     <t>Lash &amp; Brow Bar</t>
@@ -509,26 +506,26 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="11.28515625"/>
-    <col min="3" max="3" width="52.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125"/>
-    <col min="5" max="5" width="6.42578125"/>
-    <col min="6" max="6" width="10.85546875" style="1"/>
-    <col min="7" max="7" width="13.42578125"/>
-    <col min="8" max="8" width="12.85546875"/>
-    <col min="9" max="9" width="26.140625"/>
-    <col min="10" max="10" width="16.85546875"/>
-    <col min="11" max="11" width="10.140625"/>
-    <col min="12" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="11.5546875"/>
+    <col min="2" max="2" width="11.33203125"/>
+    <col min="3" max="3" width="52.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625"/>
+    <col min="5" max="5" width="6.44140625"/>
+    <col min="6" max="6" width="10.88671875" style="1"/>
+    <col min="7" max="7" width="13.44140625"/>
+    <col min="8" max="8" width="12.88671875"/>
+    <col min="9" max="9" width="26.109375"/>
+    <col min="10" max="10" width="16.88671875"/>
+    <col min="11" max="11" width="10.109375"/>
+    <col min="12" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -560,16 +557,16 @@
         <v>9</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -579,11 +576,11 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
+      <c r="D2">
+        <v>80</v>
       </c>
       <c r="E2">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="F2">
         <v>44176</v>
@@ -595,7 +592,7 @@
         <v>120344255</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2">
         <v>200</v>
@@ -610,7 +607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -618,7 +615,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -636,7 +633,7 @@
         <v>120344340</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3">
         <v>100</v>
@@ -651,31 +648,31 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C4" s="4"/>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C5" s="4"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C6" s="4"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C7" s="4"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C8" s="4"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C9" s="4"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -688,7 +685,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -701,7 +698,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -714,7 +711,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -727,7 +724,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -740,7 +737,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -753,7 +750,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -766,7 +763,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -779,7 +776,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -792,7 +789,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -805,7 +802,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -818,7 +815,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -831,7 +828,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -844,7 +841,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -857,7 +854,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -870,7 +867,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -883,7 +880,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -896,7 +893,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -909,7 +906,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -922,7 +919,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -935,7 +932,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -948,7 +945,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -961,7 +958,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -974,7 +971,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -987,7 +984,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1000,7 +997,7 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1013,7 +1010,7 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1026,7 +1023,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1039,7 +1036,7 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1052,7 +1049,7 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1065,7 +1062,7 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1078,7 +1075,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1091,22 +1088,22 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F42"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F43"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F44"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F45"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F46"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1126,6 +1123,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005F1A4E165AE4AA47A58D7F402C58032D" ma:contentTypeVersion="12" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="08e8f4128fe39f6c410bb3e184f6b02c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a770380-a541-49fb-a5e7-be562a0ab7fc" xmlns:ns3="ce6e5384-3d40-41c8-8f4c-f6763c848ff7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="638cd77b2c67c1f99ba832209e451d50" ns2:_="" ns3:_="">
     <xsd:import namespace="1a770380-a541-49fb-a5e7-be562a0ab7fc"/>
@@ -1342,22 +1354,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAF11026-BEE7-4810-A662-14866A3103A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3EC323E-1C66-4DED-84F7-F717AC772B25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B07BBEF-B0C4-4366-A071-C1C9ADEA7D0F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1374,21 +1388,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3EC323E-1C66-4DED-84F7-F717AC772B25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAF11026-BEE7-4810-A662-14866A3103A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>